<commit_message>
Add the script TST1037.
</commit_message>
<xml_diff>
--- a/NformTester/NformTester/Keywordscripts/TST983_UsersGroupManagement.xlsx
+++ b/NformTester/NformTester/Keywordscripts/TST983_UsersGroupManagement.xlsx
@@ -4696,7 +4696,7 @@
   <dimension ref="A1:O80"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="E83" sqref="E83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6607,7 +6607,7 @@
         <v>792</v>
       </c>
       <c r="F71" s="4">
-        <v>60</v>
+        <v>5</v>
       </c>
       <c r="G71" s="4"/>
       <c r="H71" s="4"/>
@@ -6668,7 +6668,7 @@
         <v>73</v>
       </c>
       <c r="D74" s="14" t="s">
-        <v>810</v>
+        <v>797</v>
       </c>
       <c r="E74" s="12" t="s">
         <v>19</v>
@@ -6855,7 +6855,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D34:D43 D50:D53 D45:D48 D3:D4 D6:D12 D14:D32 D73:D80 D55:D69 D71">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D34:D43 D73:D80 D55:D69 D71 D14:D32 D6:D12 D3:D4 D45:D48 D50:D53">
       <formula1>"C,F,T,;"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F80">

</xml_diff>